<commit_message>
'Worked on testing testConfig parameter limits'
</commit_message>
<xml_diff>
--- a/pcbs/purchaseRecs/purRec_Mouser_01.24.2012.xlsx
+++ b/pcbs/purchaseRecs/purRec_Mouser_01.24.2012.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,163 +21,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+  <si>
+    <t>Mfg Part Number</t>
+  </si>
+  <si>
+    <t>Quantity 1</t>
+  </si>
+  <si>
+    <t>Price 1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mouser Part Number</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Lead Time</t>
+  </si>
+  <si>
+    <t>Min\Mult</t>
+  </si>
+  <si>
+    <t>RoHS</t>
+  </si>
+  <si>
+    <t>PB Free</t>
+  </si>
+  <si>
+    <t>Package Type</t>
+  </si>
+  <si>
+    <t>Package Quantity</t>
+  </si>
+  <si>
+    <t>NCNR</t>
+  </si>
   <si>
     <t>Mfg Name</t>
   </si>
   <si>
+    <t>Customer Part Number</t>
+  </si>
+  <si>
+    <t>Quantity 2</t>
+  </si>
+  <si>
+    <t>Quantity 3</t>
+  </si>
+  <si>
+    <t>Quantity 4</t>
+  </si>
+  <si>
+    <t>Quantity 5</t>
+  </si>
+  <si>
+    <t>Price 2</t>
+  </si>
+  <si>
     <t>Price 3</t>
   </si>
   <si>
-    <t>579-93LC66BT-I/OT</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Standard LED - SMD Standard LED - SMD YelGrn Water Clr 60mcd 575nm</t>
-  </si>
-  <si>
-    <t>556-ATXMEGA64A3-AUR</t>
-  </si>
-  <si>
-    <t>PB Free</t>
-  </si>
-  <si>
-    <t>Microcontrollers (MCU) Microcontrollers (MCU) 8/16 bit 1.6V-3.6V 64KB + 4KB</t>
-  </si>
-  <si>
-    <t>NCNR</t>
-  </si>
-  <si>
-    <t>RoHS</t>
-  </si>
-  <si>
-    <t>Quantity 3</t>
-  </si>
-  <si>
-    <t>Package Quantity</t>
-  </si>
-  <si>
-    <t>Min\Mult</t>
-  </si>
-  <si>
-    <t>Mfg Part Number</t>
-  </si>
-  <si>
-    <t>645-598-8160-107F</t>
-  </si>
-  <si>
-    <t>10 Weeks</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>556-ATXMEGA64A3-AU</t>
-  </si>
-  <si>
-    <t>Price 2</t>
-  </si>
-  <si>
-    <t>93LC66BT-I/OT</t>
-  </si>
-  <si>
-    <t>New Product</t>
+    <t>Price 4</t>
+  </si>
+  <si>
+    <t>Price 5</t>
   </si>
   <si>
     <t>Package Price</t>
   </si>
   <si>
-    <t>Quantity 5</t>
-  </si>
-  <si>
-    <t>Quantity 1</t>
+    <t>Data Sheet URL</t>
+  </si>
+  <si>
+    <t>Lifecycle</t>
+  </si>
+  <si>
+    <t>MouseReel™</t>
+  </si>
+  <si>
+    <t>Suggested Replacement</t>
+  </si>
+  <si>
+    <t>RoHS Replacement</t>
   </si>
   <si>
     <t>598-8160-107F</t>
   </si>
   <si>
-    <t>MouseReel™</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Price 4</t>
-  </si>
-  <si>
-    <t>5 Weeks</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>Package Type</t>
-  </si>
-  <si>
-    <t>Data Sheet URL</t>
-  </si>
-  <si>
-    <t>Quantity 4</t>
-  </si>
-  <si>
-    <t>RoHS Replacement</t>
+    <t>579-93LC66BT</t>
   </si>
   <si>
     <t>ATXMEGA64A3-AU</t>
-  </si>
-  <si>
-    <t>1\1</t>
-  </si>
-  <si>
-    <t>Lead Time</t>
-  </si>
-  <si>
-    <t>Suggested Replacement</t>
-  </si>
-  <si>
-    <t>Atmel</t>
-  </si>
-  <si>
-    <t>Dialight</t>
-  </si>
-  <si>
-    <t>Mouser Part Number</t>
-  </si>
-  <si>
-    <t>Quantity 2</t>
-  </si>
-  <si>
-    <t>579-93LC66BT</t>
-  </si>
-  <si>
-    <t>Price 5</t>
-  </si>
-  <si>
-    <t>Price 1</t>
-  </si>
-  <si>
-    <t>Lifecycle</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>EEPROM EEPROM 256x16</t>
-  </si>
-  <si>
-    <t>Customer Part Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +135,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,23 +170,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -550,225 +523,132 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
       <c r="Q1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="R1" t="s">
         <v>3</v>
       </c>
       <c r="S1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="T1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="U1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="V1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>37</v>
-      </c>
       <c r="AF1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="AG1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4">
-        <v>16158</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1732</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4">
-        <v>5102</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="3">
-        <v>5.88</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>